<commit_message>
build app host FireBase add file NOTE.xlsx intruction how to deploy app to FireBase
build app host FireBase add file NOTE.xlsx intruction how to deploy app to FireBase
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\1\vue3_learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\Vue\vue3_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067C34FC-EBDB-4D4A-A36B-A8BEE900DF6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B89059D-F3D1-4E23-9105-D900980B1F10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="deploy" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -62,12 +63,27 @@
   <si>
     <t>lệnh trên để chạy server  (xem hình bên dưới)</t>
   </si>
+  <si>
+    <t>host app trên fireBase của google</t>
+  </si>
+  <si>
+    <t>https://console.firebase.google.com/?hl=vi</t>
+  </si>
+  <si>
+    <t>npm install -g firebase-tools</t>
+  </si>
+  <si>
+    <t>Fix bug :</t>
+  </si>
+  <si>
+    <t>SETTING DOMAIN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +98,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +133,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,11 +167,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,6 +349,1118 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>227047</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>141928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26A35032-3352-41DF-9CB8-62FCAD867DC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="1714500"/>
+          <a:ext cx="12419047" cy="7571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>188571</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>161286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{246D21A5-ECB3-4532-8EC5-FF5E5C12F95E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="9715500"/>
+          <a:ext cx="15428571" cy="5114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>246334</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>84996</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="36" name="Group 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6596DB0-1540-426D-BFF9-955DC31684D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2438400" y="15849600"/>
+          <a:ext cx="18534334" cy="20811396"/>
+          <a:chOff x="2381250" y="15716250"/>
+          <a:chExt cx="18534334" cy="20811396"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="34" name="Group 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5FEA6E-E8F2-4808-A9D9-129276C94AF1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2381250" y="15716250"/>
+            <a:ext cx="18534334" cy="20811396"/>
+            <a:chOff x="2409825" y="15763875"/>
+            <a:chExt cx="18534334" cy="20811396"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="30" name="Group 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37663BD9-8289-4F49-BA70-66EC30F508A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="2943225" y="29279850"/>
+              <a:ext cx="13715529" cy="7295421"/>
+              <a:chOff x="2600325" y="29527500"/>
+              <a:chExt cx="13715529" cy="7295421"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="17" name="Picture 16">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F069EE95-0A7C-4166-96A0-79206995C866}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="2628900" y="29527500"/>
+                <a:ext cx="8914286" cy="2161905"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="25" name="Group 24">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5639199E-8EE1-400A-9808-D31A69107C25}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="2600325" y="30994350"/>
+                <a:ext cx="13715529" cy="5828571"/>
+                <a:chOff x="2390775" y="30784800"/>
+                <a:chExt cx="13715529" cy="5828571"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:pic>
+              <xdr:nvPicPr>
+                <xdr:cNvPr id="19" name="Picture 18">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74E5E98-14A4-4D1F-BF5F-5513B496E722}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvPicPr>
+                  <a:picLocks noChangeAspect="1"/>
+                </xdr:cNvPicPr>
+              </xdr:nvPicPr>
+              <xdr:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </xdr:blipFill>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="12334875" y="30784800"/>
+                  <a:ext cx="3771429" cy="5828571"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+              </xdr:spPr>
+            </xdr:pic>
+            <xdr:pic>
+              <xdr:nvPicPr>
+                <xdr:cNvPr id="20" name="Picture 19">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF87F473-9819-493F-B4E9-0DA248455EBD}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvPicPr>
+                  <a:picLocks noChangeAspect="1"/>
+                </xdr:cNvPicPr>
+              </xdr:nvPicPr>
+              <xdr:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </xdr:blipFill>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="2390775" y="32156400"/>
+                  <a:ext cx="8923809" cy="2228571"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+              </xdr:spPr>
+            </xdr:pic>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE014EAA-01BA-445E-8498-D968CA8AAC2A}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvCxnSpPr>
+                  <a:endCxn id="19" idx="1"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm flipV="1">
+                  <a:off x="8172450" y="33699086"/>
+                  <a:ext cx="4162425" cy="133714"/>
+                </a:xfrm>
+                <a:prstGeom prst="straightConnector1">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:tailEnd type="triangle"/>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="3">
+                  <a:schemeClr val="accent2"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent2"/>
+                </a:fillRef>
+                <a:effectRef idx="2">
+                  <a:schemeClr val="accent2"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+          </xdr:grpSp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="33" name="Group 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5345EAE5-599C-4C61-9207-8AADCD956A9A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="2409825" y="15763875"/>
+              <a:ext cx="18534334" cy="13382594"/>
+              <a:chOff x="2409825" y="15763875"/>
+              <a:chExt cx="18534334" cy="13382594"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="29" name="Group 28">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DEE799C-54B5-4618-918C-D92382DD39BB}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="2409825" y="15763875"/>
+                <a:ext cx="18534334" cy="13029924"/>
+                <a:chOff x="1943100" y="16040100"/>
+                <a:chExt cx="18534334" cy="13029924"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:pic>
+              <xdr:nvPicPr>
+                <xdr:cNvPr id="6" name="Picture 5">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A606EE01-8B49-4A94-8FFD-9A8E562BAEB8}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvPicPr>
+                  <a:picLocks noChangeAspect="1"/>
+                </xdr:cNvPicPr>
+              </xdr:nvPicPr>
+              <xdr:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </xdr:blipFill>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="1943100" y="16040100"/>
+                  <a:ext cx="7780952" cy="3819048"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+              </xdr:spPr>
+            </xdr:pic>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="28" name="Group 27">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0200506-17CA-4A0D-AB15-AB69E7C578DF}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="1990725" y="20183475"/>
+                  <a:ext cx="18486709" cy="8886549"/>
+                  <a:chOff x="2419350" y="19745325"/>
+                  <a:chExt cx="18486709" cy="8886549"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:grpSp>
+                <xdr:nvGrpSpPr>
+                  <xdr:cNvPr id="26" name="Group 25">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC7E3C21-A085-423D-A6DF-9FC4384D2082}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvGrpSpPr/>
+                </xdr:nvGrpSpPr>
+                <xdr:grpSpPr>
+                  <a:xfrm>
+                    <a:off x="2419350" y="19745325"/>
+                    <a:ext cx="18486709" cy="8886549"/>
+                    <a:chOff x="2428875" y="19773900"/>
+                    <a:chExt cx="18486709" cy="8886549"/>
+                  </a:xfrm>
+                </xdr:grpSpPr>
+                <xdr:pic>
+                  <xdr:nvPicPr>
+                    <xdr:cNvPr id="7" name="Picture 6">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC34FDBB-5C57-41D3-A994-0C5B5BEE101F}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvPicPr>
+                      <a:picLocks noChangeAspect="1"/>
+                    </xdr:cNvPicPr>
+                  </xdr:nvPicPr>
+                  <xdr:blipFill>
+                    <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+                    <a:stretch>
+                      <a:fillRect/>
+                    </a:stretch>
+                  </xdr:blipFill>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="2428875" y="19773900"/>
+                      <a:ext cx="7209524" cy="3514286"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </xdr:spPr>
+                </xdr:pic>
+                <xdr:pic>
+                  <xdr:nvPicPr>
+                    <xdr:cNvPr id="8" name="Picture 7">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAD11BAF-48D1-4442-9169-AA085683DE39}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvPicPr>
+                      <a:picLocks noChangeAspect="1"/>
+                    </xdr:cNvPicPr>
+                  </xdr:nvPicPr>
+                  <xdr:blipFill>
+                    <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+                    <a:stretch>
+                      <a:fillRect/>
+                    </a:stretch>
+                  </xdr:blipFill>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="10344150" y="20012025"/>
+                      <a:ext cx="10400000" cy="2209524"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </xdr:spPr>
+                </xdr:pic>
+                <xdr:cxnSp macro="">
+                  <xdr:nvCxnSpPr>
+                    <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73EEF19E-1470-42D6-8FAA-805D457349EB}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvCxnSpPr>
+                      <a:endCxn id="8" idx="1"/>
+                    </xdr:cNvCxnSpPr>
+                  </xdr:nvCxnSpPr>
+                  <xdr:spPr>
+                    <a:xfrm flipV="1">
+                      <a:off x="6496050" y="21116787"/>
+                      <a:ext cx="3848100" cy="209688"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="straightConnector1">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:tailEnd type="triangle"/>
+                    </a:ln>
+                  </xdr:spPr>
+                  <xdr:style>
+                    <a:lnRef idx="3">
+                      <a:schemeClr val="accent2"/>
+                    </a:lnRef>
+                    <a:fillRef idx="0">
+                      <a:schemeClr val="accent2"/>
+                    </a:fillRef>
+                    <a:effectRef idx="2">
+                      <a:schemeClr val="accent2"/>
+                    </a:effectRef>
+                    <a:fontRef idx="minor">
+                      <a:schemeClr val="tx1"/>
+                    </a:fontRef>
+                  </xdr:style>
+                </xdr:cxnSp>
+                <xdr:pic>
+                  <xdr:nvPicPr>
+                    <xdr:cNvPr id="12" name="Picture 11">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F459ABC-B008-4FB9-AA47-D02732B8F353}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvPicPr>
+                      <a:picLocks noChangeAspect="1"/>
+                    </xdr:cNvPicPr>
+                  </xdr:nvPicPr>
+                  <xdr:blipFill>
+                    <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+                    <a:stretch>
+                      <a:fillRect/>
+                    </a:stretch>
+                  </xdr:blipFill>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="10391775" y="22783800"/>
+                      <a:ext cx="10523809" cy="2190476"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </xdr:spPr>
+                </xdr:pic>
+                <xdr:pic>
+                  <xdr:nvPicPr>
+                    <xdr:cNvPr id="13" name="Picture 12">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D5FFFA-D68B-4DF8-AD3F-027C5472385D}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvPicPr>
+                      <a:picLocks noChangeAspect="1"/>
+                    </xdr:cNvPicPr>
+                  </xdr:nvPicPr>
+                  <xdr:blipFill>
+                    <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+                    <a:stretch>
+                      <a:fillRect/>
+                    </a:stretch>
+                  </xdr:blipFill>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="2533650" y="26450925"/>
+                      <a:ext cx="10761905" cy="2209524"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </xdr:spPr>
+                </xdr:pic>
+                <xdr:cxnSp macro="">
+                  <xdr:nvCxnSpPr>
+                    <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B724A9B1-06E3-4884-A861-309624F72389}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvCxnSpPr>
+                      <a:endCxn id="13" idx="0"/>
+                    </xdr:cNvCxnSpPr>
+                  </xdr:nvCxnSpPr>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="4448175" y="22783800"/>
+                      <a:ext cx="3466428" cy="3667125"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="straightConnector1">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:tailEnd type="triangle"/>
+                    </a:ln>
+                  </xdr:spPr>
+                  <xdr:style>
+                    <a:lnRef idx="3">
+                      <a:schemeClr val="accent2"/>
+                    </a:lnRef>
+                    <a:fillRef idx="0">
+                      <a:schemeClr val="accent2"/>
+                    </a:fillRef>
+                    <a:effectRef idx="2">
+                      <a:schemeClr val="accent2"/>
+                    </a:effectRef>
+                    <a:fontRef idx="minor">
+                      <a:schemeClr val="tx1"/>
+                    </a:fontRef>
+                  </xdr:style>
+                </xdr:cxnSp>
+              </xdr:grpSp>
+              <xdr:pic>
+                <xdr:nvPicPr>
+                  <xdr:cNvPr id="27" name="Picture 26">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D503DAF-025B-4C54-B9D1-09318AC80C41}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvPicPr>
+                    <a:picLocks noChangeAspect="1"/>
+                  </xdr:cNvPicPr>
+                </xdr:nvPicPr>
+                <xdr:blipFill>
+                  <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+                  <a:stretch>
+                    <a:fillRect/>
+                  </a:stretch>
+                </xdr:blipFill>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="4343400" y="25707975"/>
+                    <a:ext cx="2847619" cy="609524"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </xdr:spPr>
+              </xdr:pic>
+            </xdr:grpSp>
+          </xdr:grpSp>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="32" name="Picture 31">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A0EE3B-D597-4D3E-861C-D652ECBF1477}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="2752725" y="28898850"/>
+                <a:ext cx="6923809" cy="247619"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="35" name="Picture 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D26F00E-AF1B-439B-BBE3-26BC0391FC7D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10306050" y="22459950"/>
+            <a:ext cx="5047619" cy="342857"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>474407</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>180074</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="44" name="Group 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A73EC849-8A6A-4B96-9D26-6356CF5FE219}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2800350" y="37747575"/>
+          <a:ext cx="14742857" cy="12972149"/>
+          <a:chOff x="2314575" y="37947600"/>
+          <a:chExt cx="14742857" cy="12972149"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="42" name="Group 41">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E281A13-4BBA-4C2B-975F-9C8C7043F6BF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2562225" y="37947600"/>
+            <a:ext cx="12172488" cy="5428951"/>
+            <a:chOff x="2428875" y="37404675"/>
+            <a:chExt cx="12172488" cy="5428951"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="39" name="Group 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33A31C6D-24D4-4569-B564-CDD5787EA207}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="2428875" y="37404675"/>
+              <a:ext cx="12172488" cy="2390571"/>
+              <a:chOff x="2428875" y="37404675"/>
+              <a:chExt cx="12172488" cy="2390571"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="31" name="Picture 30">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CD4935-E67A-4EEA-99F5-445796E5A1CA}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="2428875" y="37404675"/>
+                <a:ext cx="8295238" cy="2390476"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="37" name="Picture 36">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E805F3D8-DA1D-4B63-AFAE-E24850ECDEEF}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10963275" y="38166675"/>
+                <a:ext cx="3533333" cy="1628571"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="38" name="Picture 37">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F41B627-3EEE-4AFE-9CBC-2DC177082965}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10906125" y="37652325"/>
+                <a:ext cx="3695238" cy="333333"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+        </xdr:grpSp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="41" name="Picture 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB71DAB-85B3-401F-A734-0DBA643F27B3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2438400" y="40443150"/>
+              <a:ext cx="9323809" cy="2390476"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="43" name="Picture 42">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C17167DF-C04E-4FF8-83C9-970955BA0358}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2314575" y="43710225"/>
+            <a:ext cx="14742857" cy="7209524"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>531892</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>161595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590D7AD0-2F34-48D4-BB94-2D29861D58D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="53349525"/>
+          <a:ext cx="12066667" cy="2638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>408076</xdr:colOff>
+      <xdr:row>323</xdr:row>
+      <xdr:rowOff>142238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F447B9A9-6339-47A9-81E5-CB3BD9BE002F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="56778525"/>
+          <a:ext cx="11990476" cy="5095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>300</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>332490</xdr:colOff>
+      <xdr:row>325</xdr:row>
+      <xdr:rowOff>66081</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E65389-CED5-401F-BC6C-757C63B13684}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15201900" y="57426225"/>
+          <a:ext cx="7076190" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>329</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>494476</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>18333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A006E5CE-410E-46C7-B9F4-457DEEA92973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3657600" y="62874525"/>
+          <a:ext cx="6590476" cy="5733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -552,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D12:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +1877,7 @@
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="1"/>
@@ -847,4 +2026,144 @@
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318C9C8-0CC5-483B-8E19-6F0798D5D900}">
+  <dimension ref="B6:Y276"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C313" workbookViewId="0">
+      <selection activeCell="U334" sqref="U334"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E83" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+    </row>
+    <row r="119" spans="18:25" x14ac:dyDescent="0.25">
+      <c r="R119" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T119" s="6"/>
+      <c r="U119" s="6"/>
+      <c r="V119" s="6"/>
+      <c r="W119" s="6"/>
+      <c r="X119" s="6"/>
+      <c r="Y119" s="6"/>
+    </row>
+    <row r="134" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+      <c r="M134" s="8"/>
+    </row>
+    <row r="135" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+      <c r="M135" s="8"/>
+    </row>
+    <row r="136" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="8"/>
+    </row>
+    <row r="137" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="8"/>
+    </row>
+    <row r="138" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H138" s="9"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="9"/>
+      <c r="K138" s="9"/>
+      <c r="L138" s="9"/>
+      <c r="M138" s="8"/>
+    </row>
+    <row r="153" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6"/>
+      <c r="L153" s="6"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6"/>
+      <c r="P153" s="6"/>
+    </row>
+    <row r="197" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S197" s="8"/>
+      <c r="T197" s="8"/>
+      <c r="U197" s="8"/>
+      <c r="V197" s="8"/>
+      <c r="W197" s="8"/>
+      <c r="X197" s="8"/>
+      <c r="Y197" s="8"/>
+    </row>
+    <row r="198" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S198" s="8"/>
+      <c r="T198" s="8"/>
+      <c r="U198" s="8"/>
+      <c r="V198" s="8"/>
+      <c r="W198" s="8"/>
+      <c r="X198" s="8"/>
+      <c r="Y198" s="8"/>
+    </row>
+    <row r="199" spans="19:25" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="S199" s="10"/>
+      <c r="T199" s="11"/>
+      <c r="U199" s="11"/>
+      <c r="V199" s="11"/>
+      <c r="W199" s="11"/>
+      <c r="X199" s="11"/>
+      <c r="Y199" s="8"/>
+    </row>
+    <row r="276" spans="6:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="F276" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G276" s="12"/>
+      <c r="H276" s="12"/>
+      <c r="I276" s="12"/>
+      <c r="J276" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
show detail, delete image, set rules in FireBase
show detail, delete image, set rules in FireBase
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\Vue\vue3_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B89059D-F3D1-4E23-9105-D900980B1F10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634BF7B8-E653-4125-8744-A257868550F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -77,13 +77,43 @@
   </si>
   <si>
     <t>SETTING DOMAIN</t>
+  </si>
+  <si>
+    <t>RULES FIREBASE</t>
+  </si>
+  <si>
+    <t>rules_version = '2';</t>
+  </si>
+  <si>
+    <t>service cloud.firestore {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  match /databases/{database}/documents {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    match /playlists/{docId} {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      allow read, create: if request.auth != null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      allow delete, update: if request.auth.uid == resource.data.userId;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +146,20 @@
     </font>
     <font>
       <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -167,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -181,6 +225,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1463,6 +1509,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>512762</xdr:colOff>
+      <xdr:row>399</xdr:row>
+      <xdr:rowOff>132559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B10D9EE8-E661-42C1-952C-4C24CBC2126F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3657600" y="70589775"/>
+          <a:ext cx="12704762" cy="6323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2030,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318C9C8-0CC5-483B-8E19-6F0798D5D900}">
-  <dimension ref="B6:Y276"/>
+  <dimension ref="B6:Y413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C313" workbookViewId="0">
-      <selection activeCell="U334" sqref="U334"/>
+    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="H407" sqref="H407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,6 +2251,156 @@
       <c r="I276" s="12"/>
       <c r="J276" s="12"/>
     </row>
+    <row r="367" spans="7:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G367" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H367" s="14"/>
+      <c r="I367" s="14"/>
+    </row>
+    <row r="368" spans="7:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G368" s="13"/>
+      <c r="H368" s="13"/>
+      <c r="I368" s="13"/>
+    </row>
+    <row r="369" spans="7:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G369" s="13"/>
+      <c r="H369" s="13"/>
+      <c r="I369" s="13"/>
+    </row>
+    <row r="370" spans="7:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G370" s="13"/>
+      <c r="H370" s="13"/>
+      <c r="I370" s="13"/>
+    </row>
+    <row r="403" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P403" s="4"/>
+      <c r="Q403" s="4"/>
+      <c r="R403" s="4"/>
+      <c r="S403" s="4"/>
+      <c r="T403" s="4"/>
+      <c r="U403" s="4"/>
+      <c r="V403" s="4"/>
+      <c r="W403" s="4"/>
+    </row>
+    <row r="404" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P404" s="4"/>
+      <c r="Q404" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R404" s="4"/>
+      <c r="S404" s="4"/>
+      <c r="T404" s="4"/>
+      <c r="U404" s="4"/>
+      <c r="V404" s="4"/>
+      <c r="W404" s="4"/>
+    </row>
+    <row r="405" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P405" s="4"/>
+      <c r="Q405" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R405" s="4"/>
+      <c r="S405" s="4"/>
+      <c r="T405" s="4"/>
+      <c r="U405" s="4"/>
+      <c r="V405" s="4"/>
+      <c r="W405" s="4"/>
+    </row>
+    <row r="406" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P406" s="4"/>
+      <c r="Q406" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R406" s="4"/>
+      <c r="S406" s="4"/>
+      <c r="T406" s="4"/>
+      <c r="U406" s="4"/>
+      <c r="V406" s="4"/>
+      <c r="W406" s="4"/>
+    </row>
+    <row r="407" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P407" s="4"/>
+      <c r="Q407" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R407" s="4"/>
+      <c r="S407" s="4"/>
+      <c r="T407" s="4"/>
+      <c r="U407" s="4"/>
+      <c r="V407" s="4"/>
+      <c r="W407" s="4"/>
+    </row>
+    <row r="408" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P408" s="4"/>
+      <c r="Q408" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R408" s="4"/>
+      <c r="S408" s="4"/>
+      <c r="T408" s="4"/>
+      <c r="U408" s="4"/>
+      <c r="V408" s="4"/>
+      <c r="W408" s="4"/>
+    </row>
+    <row r="409" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P409" s="4"/>
+      <c r="Q409" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R409" s="4"/>
+      <c r="S409" s="4"/>
+      <c r="T409" s="4"/>
+      <c r="U409" s="4"/>
+      <c r="V409" s="4"/>
+      <c r="W409" s="4"/>
+    </row>
+    <row r="410" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P410" s="4"/>
+      <c r="Q410" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R410" s="4"/>
+      <c r="S410" s="4"/>
+      <c r="T410" s="4"/>
+      <c r="U410" s="4"/>
+      <c r="V410" s="4"/>
+      <c r="W410" s="4"/>
+    </row>
+    <row r="411" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P411" s="4"/>
+      <c r="Q411" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R411" s="4"/>
+      <c r="S411" s="4"/>
+      <c r="T411" s="4"/>
+      <c r="U411" s="4"/>
+      <c r="V411" s="4"/>
+      <c r="W411" s="4"/>
+    </row>
+    <row r="412" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P412" s="4"/>
+      <c r="Q412" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R412" s="4"/>
+      <c r="S412" s="4"/>
+      <c r="T412" s="4"/>
+      <c r="U412" s="4"/>
+      <c r="V412" s="4"/>
+      <c r="W412" s="4"/>
+    </row>
+    <row r="413" spans="16:23" x14ac:dyDescent="0.25">
+      <c r="P413" s="4"/>
+      <c r="Q413" s="4"/>
+      <c r="R413" s="4"/>
+      <c r="S413" s="4"/>
+      <c r="T413" s="4"/>
+      <c r="U413" s="4"/>
+      <c r="V413" s="4"/>
+      <c r="W413" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
delete, update Document FireBase
delete, update Document FireBase
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\Vue\vue3_learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\1\vue3_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634BF7B8-E653-4125-8744-A257868550F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E687BD-0759-4AA6-A3C5-1562CE6A303B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">      allow delete, update: if request.auth.uid == resource.data.userId;</t>
+  </si>
+  <si>
+    <t>// https://firebase.google.com/docs/firestore/query-data/queries</t>
+  </si>
+  <si>
+    <t>RULES THAM KHẢO CODING</t>
   </si>
 </sst>
 </file>
@@ -2120,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318C9C8-0CC5-483B-8E19-6F0798D5D900}">
-  <dimension ref="B6:Y413"/>
+  <dimension ref="B6:Y421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="H407" sqref="H407"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="H414" sqref="H414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,6 +2407,16 @@
       <c r="V413" s="4"/>
       <c r="W413" s="4"/>
     </row>
+    <row r="419" spans="6:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="F419" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="421" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F421" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>